<commit_message>
better path handling on windows
used os.path.abspath to (hopefully) have better drap and drop handling
on windows machines
</commit_message>
<xml_diff>
--- a/D47_Temperature_calibrations_for_John.xlsx
+++ b/D47_Temperature_calibrations_for_John.xlsx
@@ -88,8 +88,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -100,13 +102,15 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,7 +443,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -469,11 +473,11 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>0.35199999999999998</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="B2">
         <f>SQRT(1000000/((-0.03069343+SQRT(0.03069343^2-4*0.00074611*(0.20083726-A2)))/(2*0.00074611)))-273.15</f>
-        <v>201.17803880249119</v>
+        <v>367.68986452578611</v>
       </c>
       <c r="E2">
         <v>7.4611471900000003E-4</v>
@@ -483,6 +487,15 @@
       </c>
       <c r="G2">
         <v>0.200837260854</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>0.245</v>
+      </c>
+      <c r="B3">
+        <f>SQRT(1000000/((-0.03069343+SQRT(0.03069343^2-4*0.00074611*(0.20083726-A3)))/(2*0.00074611)))-273.15</f>
+        <v>574.50580292734196</v>
       </c>
     </row>
     <row r="5" spans="1:7">

</xml_diff>